<commit_message>
added code for mobile RKA
</commit_message>
<xml_diff>
--- a/src/test/resources/features/PageVerification/MobileWebLocatorsMapping.xlsx
+++ b/src/test/resources/features/PageVerification/MobileWebLocatorsMapping.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Academy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raharya\Desktop\Cart_Po_MOB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12915" windowHeight="5100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CartVerification" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="159">
   <si>
     <t>|SignInPage_EmailAddress_txt</t>
   </si>
@@ -297,6 +298,211 @@
   </si>
   <si>
     <t>Xpath in Mobile</t>
+  </si>
+  <si>
+    <t>Xpath for Mobile</t>
+  </si>
+  <si>
+    <t>|# Verify following elements in Cart page "Your Cart "|</t>
+  </si>
+  <si>
+    <t>|ContinueShopping_Link|</t>
+  </si>
+  <si>
+    <t>|YourCart_Header|</t>
+  </si>
+  <si>
+    <t>|Items_txt|</t>
+  </si>
+  <si>
+    <t>|TotalYourCart_txt|</t>
+  </si>
+  <si>
+    <t>|checkOutYourCart_Btn|</t>
+  </si>
+  <si>
+    <t>Different</t>
+  </si>
+  <si>
+    <t>|# Verify following elements in Cart page "Your Cart item details "|</t>
+  </si>
+  <si>
+    <t>|Image_ITemInCart|</t>
+  </si>
+  <si>
+    <t>|CartProductName_Link   |</t>
+  </si>
+  <si>
+    <t>|color_input_txt       |</t>
+  </si>
+  <si>
+    <t>|Size_input_txt|</t>
+  </si>
+  <si>
+    <t>|ShipToMe_radioBtn|</t>
+  </si>
+  <si>
+    <t>|InStorePickup_FREE_radioBtn |</t>
+  </si>
+  <si>
+    <t>|Quantity_input_txt|</t>
+  </si>
+  <si>
+    <t>|Quantity_txt|</t>
+  </si>
+  <si>
+    <t>|toolTip_icon|</t>
+  </si>
+  <si>
+    <t>|AddToWishList_btn|</t>
+  </si>
+  <si>
+    <t>|RemoveFromCart_Btn|</t>
+  </si>
+  <si>
+    <t>|CartItemAmount_txt|</t>
+  </si>
+  <si>
+    <t>|Color_txt|</t>
+  </si>
+  <si>
+    <t>|Size_txt|</t>
+  </si>
+  <si>
+    <t>|EstArrival_txt|</t>
+  </si>
+  <si>
+    <t>|# Verify following elements in Cart page"Order Summary"|</t>
+  </si>
+  <si>
+    <t>|OrderSummary_Header|</t>
+  </si>
+  <si>
+    <t>|Plus_AddPromoCode_btn|</t>
+  </si>
+  <si>
+    <t>|Minus_HidePromo_btn|</t>
+  </si>
+  <si>
+    <t>|EnterPromoCode_input|</t>
+  </si>
+  <si>
+    <t>|Submit_PromoCode_btn|</t>
+  </si>
+  <si>
+    <t>|checkOut_OrderSummary_btn|</t>
+  </si>
+  <si>
+    <t>|Total_txt|</t>
+  </si>
+  <si>
+    <t>|SubTotal_txt|</t>
+  </si>
+  <si>
+    <t>|EstimatedShipping_txt|</t>
+  </si>
+  <si>
+    <t>|EstimatedTaxes_txt|</t>
+  </si>
+  <si>
+    <t>|ZipCode_txt|</t>
+  </si>
+  <si>
+    <t>|# Verify following elements in Cart page"We Accept"|</t>
+  </si>
+  <si>
+    <t>|Visa_img|</t>
+  </si>
+  <si>
+    <t>|MasterCard_img|</t>
+  </si>
+  <si>
+    <t>|Paypal_img|</t>
+  </si>
+  <si>
+    <t>|GooglePay_img|</t>
+  </si>
+  <si>
+    <t>|ApplePay_img|</t>
+  </si>
+  <si>
+    <t>|AmericanExpress_img|</t>
+  </si>
+  <si>
+    <t>|Discover_img|</t>
+  </si>
+  <si>
+    <t>|# Verify following elements in Cart page"Free In Store Return"|</t>
+  </si>
+  <si>
+    <t>|FreeInStoreReturns_txt|</t>
+  </si>
+  <si>
+    <t>|ShippingPolicy_link|</t>
+  </si>
+  <si>
+    <t>|ReturnPolicy_link|</t>
+  </si>
+  <si>
+    <t>|# Verify following elements in Cart page"Shop With Confidance"|</t>
+  </si>
+  <si>
+    <t>|ShopWithConfidance_txt|</t>
+  </si>
+  <si>
+    <t>|# Verify following elements in Cart page"Calculate Shipping"|</t>
+  </si>
+  <si>
+    <t>|ZipCode_input_txt|</t>
+  </si>
+  <si>
+    <t>|Submit_CalculateShipping_btn|</t>
+  </si>
+  <si>
+    <t>|CalculateShipping_txt|</t>
+  </si>
+  <si>
+    <t>|EnterYourZIPcodeforShippingCost_txt|</t>
+  </si>
+  <si>
+    <t>|X_btn|</t>
+  </si>
+  <si>
+    <t>|# Verify following elements in Cart page
+"After clicking on  Shiping Policy"|</t>
+  </si>
+  <si>
+    <t>|ShippingCharges_header|</t>
+  </si>
+  <si>
+    <t>|# Verify following elements in Cart page"When cart is empty"|</t>
+  </si>
+  <si>
+    <t>|YourCartIsEmpty_Txt|</t>
+  </si>
+  <si>
+    <t>|SignIn_btn|</t>
+  </si>
+  <si>
+    <t>|ContinueShopping_btn|</t>
+  </si>
+  <si>
+    <t>|ContinueShopping_forEmptyCart_Link|</t>
+  </si>
+  <si>
+    <t>|# Verify following elements in Cart page"PromoCode"|</t>
+  </si>
+  <si>
+    <t>|Promocode_Price_txt|</t>
+  </si>
+  <si>
+    <t>|InvalidPromocode_txt|</t>
+  </si>
+  <si>
+    <t>|Promocode_Txt|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Element name  </t>
   </si>
 </sst>
 </file>
@@ -333,7 +539,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +555,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -389,6 +607,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,7 +894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1395,4 +1618,565 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated checkout page verification
</commit_message>
<xml_diff>
--- a/src/test/resources/features/PageVerification/MobileWebLocatorsMapping.xlsx
+++ b/src/test/resources/features/PageVerification/MobileWebLocatorsMapping.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="269">
   <si>
     <t>|SignInPage_EmailAddress_txt</t>
   </si>
@@ -656,9 +656,6 @@
     <t>|Total_price|</t>
   </si>
   <si>
-    <t>Not found this element</t>
-  </si>
-  <si>
     <t>|#%%%%%  ITems under Order Summary  %%%%%|</t>
   </si>
   <si>
@@ -812,9 +809,6 @@
     <t>|ZipCode_Input|</t>
   </si>
   <si>
-    <t>|Payment_Input|</t>
-  </si>
-  <si>
     <t>|State_DD|</t>
   </si>
   <si>
@@ -836,7 +830,10 @@
     <t>|PayPalCheckOut_Btn|</t>
   </si>
   <si>
-    <t>Elements hidden - Defect raised</t>
+    <t>City_Input|</t>
+  </si>
+  <si>
+    <t>Element not found</t>
   </si>
 </sst>
 </file>
@@ -2599,8 +2596,8 @@
   <dimension ref="A1:C118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B111" sqref="B111"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2956,7 +2953,7 @@
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>209</v>
+        <v>268</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2965,7 +2962,7 @@
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>209</v>
+        <v>268</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2992,7 +2989,7 @@
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>209</v>
+        <v>268</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3001,7 +2998,7 @@
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
-        <v>209</v>
+        <v>268</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -3042,25 +3039,25 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B60" s="6"/>
       <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>6</v>
@@ -3069,7 +3066,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>6</v>
@@ -3078,7 +3075,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>6</v>
@@ -3087,7 +3084,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>6</v>
@@ -3096,7 +3093,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>6</v>
@@ -3105,7 +3102,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>6</v>
@@ -3114,7 +3111,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>6</v>
@@ -3123,7 +3120,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>6</v>
@@ -3132,7 +3129,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>6</v>
@@ -3141,7 +3138,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>6</v>
@@ -3150,32 +3147,30 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B74" s="6"/>
       <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>6</v>
@@ -3184,7 +3179,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>6</v>
@@ -3193,7 +3188,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>6</v>
@@ -3202,7 +3197,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>6</v>
@@ -3211,7 +3206,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>6</v>
@@ -3220,7 +3215,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>6</v>
@@ -3229,7 +3224,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>6</v>
@@ -3238,7 +3233,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>6</v>
@@ -3247,7 +3242,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>6</v>
@@ -3256,7 +3251,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>6</v>
@@ -3265,7 +3260,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>6</v>
@@ -3274,14 +3269,14 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B87" s="16"/>
       <c r="C87" s="1"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>6</v>
@@ -3290,7 +3285,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>6</v>
@@ -3299,7 +3294,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>6</v>
@@ -3308,7 +3303,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>6</v>
@@ -3317,7 +3312,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>6</v>
@@ -3326,7 +3321,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>6</v>
@@ -3335,7 +3330,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>6</v>
@@ -3344,7 +3339,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>6</v>
@@ -3353,7 +3348,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>6</v>
@@ -3362,7 +3357,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>6</v>
@@ -3371,7 +3366,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>6</v>
@@ -3380,14 +3375,14 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B99" s="16"/>
       <c r="C99" s="1"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>6</v>
@@ -3396,7 +3391,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>6</v>
@@ -3405,7 +3400,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>6</v>
@@ -3414,7 +3409,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>6</v>
@@ -3423,7 +3418,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>6</v>
@@ -3432,7 +3427,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>6</v>
@@ -3441,7 +3436,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>6</v>
@@ -3450,16 +3445,16 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>98</v>
+        <v>256</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C107" s="1"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>98</v>
@@ -3468,7 +3463,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>6</v>
@@ -3477,7 +3472,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>6</v>
@@ -3486,74 +3481,72 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B111" s="1"/>
-      <c r="C111" s="1" t="s">
-        <v>269</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C111" s="1"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B112" s="1"/>
-      <c r="C112" s="1" t="s">
-        <v>269</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C112" s="1"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B113" s="1"/>
-      <c r="C113" s="1" t="s">
-        <v>269</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C113" s="1"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B114" s="1"/>
-      <c r="C114" s="1" t="s">
-        <v>269</v>
-      </c>
+        <v>262</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C114" s="1"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B115" s="1"/>
-      <c r="C115" s="1" t="s">
-        <v>269</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C115" s="1"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B116" s="1"/>
-      <c r="C116" s="1" t="s">
-        <v>269</v>
-      </c>
+      <c r="C116" s="1"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1" t="s">
-        <v>269</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C117" s="1"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B118" s="1"/>
+        <v>266</v>
+      </c>
+      <c r="B118" s="2"/>
       <c r="C118" s="1" t="s">
-        <v>269</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committing code for RK DKP and AK
</commit_message>
<xml_diff>
--- a/src/test/resources/features/PageVerification/MobileWebLocatorsMapping.xlsx
+++ b/src/test/resources/features/PageVerification/MobileWebLocatorsMapping.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Academy\Automation\Latest Code\qe-r2-automation-test\src\test\resources\features\PageVerification\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="5955" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="6810" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MyAccount" sheetId="1" r:id="rId1"/>
@@ -17,6 +12,7 @@
     <sheet name="Checkout" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="267">
   <si>
     <t>|SignInPage_EmailAddress_txt</t>
   </si>
@@ -695,9 +691,6 @@
     <t>|EditMyCart_Link|</t>
   </si>
   <si>
-    <t>Element locators not matching in application</t>
-  </si>
-  <si>
     <t>|# Verify following elements in Checkout page "Payment"|</t>
   </si>
   <si>
@@ -831,9 +824,6 @@
   </si>
   <si>
     <t>City_Input|</t>
-  </si>
-  <si>
-    <t>Element not found</t>
   </si>
 </sst>
 </file>
@@ -998,7 +988,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1022,6 +1012,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2596,8 +2588,8 @@
   <dimension ref="A1:C118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2951,19 +2943,19 @@
       <c r="A49" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1" t="s">
-        <v>268</v>
-      </c>
+      <c r="B49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1" t="s">
-        <v>268</v>
-      </c>
+      <c r="B50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
@@ -2987,19 +2979,19 @@
       <c r="A53" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1" t="s">
-        <v>268</v>
-      </c>
+      <c r="B53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1" t="s">
-        <v>268</v>
-      </c>
+      <c r="B54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="1"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
@@ -3048,12 +3040,10 @@
       <c r="A61" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>222</v>
-      </c>
+      <c r="B61" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
@@ -3149,28 +3139,28 @@
       <c r="A72" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B72" s="2"/>
-      <c r="C72" s="1" t="s">
-        <v>222</v>
-      </c>
+      <c r="B72" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C72" s="1"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B74" s="6"/>
       <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>6</v>
@@ -3179,7 +3169,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>6</v>
@@ -3188,7 +3178,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>6</v>
@@ -3197,7 +3187,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>6</v>
@@ -3206,7 +3196,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>6</v>
@@ -3215,7 +3205,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>6</v>
@@ -3224,7 +3214,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>6</v>
@@ -3233,7 +3223,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>6</v>
@@ -3242,7 +3232,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>6</v>
@@ -3251,7 +3241,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>6</v>
@@ -3260,7 +3250,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>6</v>
@@ -3269,14 +3259,14 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B87" s="16"/>
       <c r="C87" s="1"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>6</v>
@@ -3285,7 +3275,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>6</v>
@@ -3294,7 +3284,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>6</v>
@@ -3303,7 +3293,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>6</v>
@@ -3312,7 +3302,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>6</v>
@@ -3321,7 +3311,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>6</v>
@@ -3330,7 +3320,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>6</v>
@@ -3339,7 +3329,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>6</v>
@@ -3348,7 +3338,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>6</v>
@@ -3357,7 +3347,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>6</v>
@@ -3366,7 +3356,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>6</v>
@@ -3375,14 +3365,14 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B99" s="16"/>
       <c r="C99" s="1"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>6</v>
@@ -3391,7 +3381,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>6</v>
@@ -3400,7 +3390,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>6</v>
@@ -3409,7 +3399,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>6</v>
@@ -3418,7 +3408,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>6</v>
@@ -3427,7 +3417,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>6</v>
@@ -3436,7 +3426,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>6</v>
@@ -3445,7 +3435,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>6</v>
@@ -3454,16 +3444,16 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>98</v>
+        <v>256</v>
+      </c>
+      <c r="B108" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="C108" s="1"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>6</v>
@@ -3472,7 +3462,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>6</v>
@@ -3481,7 +3471,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>6</v>
@@ -3490,7 +3480,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>6</v>
@@ -3499,7 +3489,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>6</v>
@@ -3508,7 +3498,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>6</v>
@@ -3517,7 +3507,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>6</v>
@@ -3526,14 +3516,14 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>6</v>
@@ -3542,12 +3532,12 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B118" s="2"/>
-      <c r="C118" s="1" t="s">
-        <v>222</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="B118" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C118" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
committed scripts for PLCC-50 and came up with  backgroud clause in order to reduce number of lines in FF
</commit_message>
<xml_diff>
--- a/src/test/resources/features/PageVerification/MobileWebLocatorsMapping.xlsx
+++ b/src/test/resources/features/PageVerification/MobileWebLocatorsMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="6810" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12560" windowHeight="4950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MyAccount" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Checkout" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:E15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1006,14 +1006,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1300,14 +1300,14 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="65.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1315,13 +1315,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>89</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1361,13 +1361,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1383,13 +1383,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1440,7 +1440,7 @@
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1520,13 +1520,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="7"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -1582,13 +1582,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B37" s="7"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
@@ -1615,7 +1615,7 @@
       </c>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
@@ -1624,7 +1624,7 @@
       </c>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>38</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>39</v>
       </c>
@@ -1644,7 +1644,7 @@
       </c>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>40</v>
       </c>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>41</v>
       </c>
@@ -1662,7 +1662,7 @@
       </c>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>42</v>
       </c>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>43</v>
       </c>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>44</v>
       </c>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>45</v>
       </c>
@@ -1698,7 +1698,7 @@
       </c>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>46</v>
       </c>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>47</v>
       </c>
@@ -1716,7 +1716,7 @@
       </c>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>88</v>
       </c>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>87</v>
       </c>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>86</v>
       </c>
@@ -1743,13 +1743,13 @@
       </c>
       <c r="C54" s="1"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B56" s="7"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>50</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>51</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>52</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>53</v>
       </c>
@@ -1781,13 +1781,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B62" s="7"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>55</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>56</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>57</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>58</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>59</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>60</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>61</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>62</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>63</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>64</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>65</v>
       </c>
@@ -1875,13 +1875,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B75" s="7"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>67</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>68</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>69</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>70</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>71</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>72</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>73</v>
       </c>
@@ -1937,13 +1937,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="6" t="s">
         <v>74</v>
       </c>
       <c r="B84" s="7"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>75</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>76</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>77</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>78</v>
       </c>
@@ -1975,13 +1975,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="6" t="s">
         <v>79</v>
       </c>
       <c r="B90" s="7"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>80</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>81</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>82</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>83</v>
       </c>
@@ -2026,17 +2026,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>158</v>
       </c>
@@ -2044,13 +2044,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>92</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>93</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>94</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>95</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>96</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>97</v>
       </c>
@@ -2090,17 +2090,17 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>99</v>
       </c>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>100</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>101</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>102</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>103</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>104</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>105</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>106</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>107</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>108</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>109</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>110</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>111</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>112</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>113</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>114</v>
       </c>
@@ -2220,17 +2220,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>115</v>
       </c>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>116</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>117</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>118</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>119</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>120</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>121</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>122</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>123</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>124</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>125</v>
       </c>
@@ -2310,23 +2310,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
         <v>127</v>
       </c>
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>128</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>129</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>130</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>131</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>132</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>133</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>134</v>
       </c>
@@ -2382,17 +2382,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
         <v>135</v>
       </c>
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>136</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>137</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>138</v>
       </c>
@@ -2416,17 +2416,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>139</v>
       </c>
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>140</v>
       </c>
@@ -2434,17 +2434,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>141</v>
       </c>
       <c r="B56" s="1"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>142</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>143</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>144</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>145</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>146</v>
       </c>
@@ -2484,17 +2484,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
     </row>
-    <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
         <v>147</v>
       </c>
       <c r="B63" s="1"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>148</v>
       </c>
@@ -2502,17 +2502,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
         <v>149</v>
       </c>
       <c r="B66" s="1"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>150</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>151</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>152</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>153</v>
       </c>
@@ -2544,17 +2544,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
         <v>154</v>
       </c>
       <c r="B72" s="1"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>155</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>156</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>157</v>
       </c>
@@ -2587,19 +2587,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -2607,13 +2607,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>162</v>
       </c>
       <c r="B2" s="13"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>159</v>
       </c>
@@ -2621,13 +2621,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>160</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>161</v>
       </c>
@@ -2635,13 +2635,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>163</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>164</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>165</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>166</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>167</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>168</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>169</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>170</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>172</v>
       </c>
@@ -2705,13 +2705,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>171</v>
       </c>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>173</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>174</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>175</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>176</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>177</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>178</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>179</v>
       </c>
@@ -2767,19 +2767,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>180</v>
       </c>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="14" t="s">
         <v>171</v>
       </c>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>181</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>182</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>183</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>184</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>185</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>186</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>187</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>188</v>
       </c>
@@ -2843,13 +2843,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>189</v>
       </c>
       <c r="B36" s="6"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>190</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>191</v>
       </c>
@@ -2865,13 +2865,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="14" t="s">
         <v>171</v>
       </c>
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>192</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>193</v>
       </c>
@@ -2887,14 +2887,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
         <v>194</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>195</v>
       </c>
@@ -2903,7 +2903,7 @@
       </c>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>196</v>
       </c>
@@ -2912,7 +2912,7 @@
       </c>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>197</v>
       </c>
@@ -2921,7 +2921,7 @@
       </c>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>198</v>
       </c>
@@ -2930,7 +2930,7 @@
       </c>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>199</v>
       </c>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>200</v>
       </c>
@@ -2948,7 +2948,7 @@
       </c>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>201</v>
       </c>
@@ -2957,7 +2957,7 @@
       </c>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>202</v>
       </c>
@@ -2966,7 +2966,7 @@
       </c>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>203</v>
       </c>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>204</v>
       </c>
@@ -2984,7 +2984,7 @@
       </c>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>205</v>
       </c>
@@ -2993,7 +2993,7 @@
       </c>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>206</v>
       </c>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>207</v>
       </c>
@@ -3011,7 +3011,7 @@
       </c>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>208</v>
       </c>
@@ -3020,7 +3020,7 @@
       </c>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>122</v>
       </c>
@@ -3029,23 +3029,23 @@
       </c>
       <c r="C58" s="1"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="6" t="s">
         <v>209</v>
       </c>
       <c r="B60" s="6"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>211</v>
       </c>
@@ -3054,7 +3054,7 @@
       </c>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>212</v>
       </c>
@@ -3063,7 +3063,7 @@
       </c>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>213</v>
       </c>
@@ -3072,7 +3072,7 @@
       </c>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>214</v>
       </c>
@@ -3081,7 +3081,7 @@
       </c>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>215</v>
       </c>
@@ -3090,7 +3090,7 @@
       </c>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>216</v>
       </c>
@@ -3099,7 +3099,7 @@
       </c>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>217</v>
       </c>
@@ -3108,7 +3108,7 @@
       </c>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>218</v>
       </c>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>219</v>
       </c>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>220</v>
       </c>
@@ -3135,30 +3135,30 @@
       </c>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B72" s="18" t="s">
+      <c r="B72" s="16" t="s">
         <v>98</v>
       </c>
       <c r="C72" s="1"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="6" t="s">
         <v>222</v>
       </c>
       <c r="B74" s="6"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
         <v>223</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>224</v>
       </c>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>225</v>
       </c>
@@ -3176,7 +3176,7 @@
       </c>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>226</v>
       </c>
@@ -3185,7 +3185,7 @@
       </c>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>227</v>
       </c>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>228</v>
       </c>
@@ -3203,7 +3203,7 @@
       </c>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>229</v>
       </c>
@@ -3212,7 +3212,7 @@
       </c>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>230</v>
       </c>
@@ -3221,7 +3221,7 @@
       </c>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>231</v>
       </c>
@@ -3230,7 +3230,7 @@
       </c>
       <c r="C83" s="1"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>232</v>
       </c>
@@ -3239,7 +3239,7 @@
       </c>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>233</v>
       </c>
@@ -3248,7 +3248,7 @@
       </c>
       <c r="C85" s="1"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>234</v>
       </c>
@@ -3257,14 +3257,14 @@
       </c>
       <c r="C86" s="1"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="15" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="B87" s="16"/>
+      <c r="B87" s="18"/>
       <c r="C87" s="1"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>236</v>
       </c>
@@ -3273,7 +3273,7 @@
       </c>
       <c r="C88" s="1"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>237</v>
       </c>
@@ -3282,7 +3282,7 @@
       </c>
       <c r="C89" s="1"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>238</v>
       </c>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>239</v>
       </c>
@@ -3300,7 +3300,7 @@
       </c>
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>240</v>
       </c>
@@ -3309,7 +3309,7 @@
       </c>
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>241</v>
       </c>
@@ -3318,7 +3318,7 @@
       </c>
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>242</v>
       </c>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>243</v>
       </c>
@@ -3336,7 +3336,7 @@
       </c>
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>244</v>
       </c>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>245</v>
       </c>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>246</v>
       </c>
@@ -3363,14 +3363,14 @@
       </c>
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="15" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="B99" s="16"/>
+      <c r="B99" s="18"/>
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>248</v>
       </c>
@@ -3379,7 +3379,7 @@
       </c>
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>249</v>
       </c>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>250</v>
       </c>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>251</v>
       </c>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>252</v>
       </c>
@@ -3415,7 +3415,7 @@
       </c>
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>253</v>
       </c>
@@ -3424,7 +3424,7 @@
       </c>
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>254</v>
       </c>
@@ -3433,7 +3433,7 @@
       </c>
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
         <v>255</v>
       </c>
@@ -3442,16 +3442,16 @@
       </c>
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B108" s="17" t="s">
+      <c r="B108" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>257</v>
       </c>
@@ -3460,7 +3460,7 @@
       </c>
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>258</v>
       </c>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>266</v>
       </c>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>259</v>
       </c>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="C112" s="1"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>260</v>
       </c>
@@ -3496,7 +3496,7 @@
       </c>
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>261</v>
       </c>
@@ -3505,7 +3505,7 @@
       </c>
       <c r="C114" s="1"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>262</v>
       </c>
@@ -3514,14 +3514,14 @@
       </c>
       <c r="C115" s="1"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>263</v>
       </c>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>264</v>
       </c>
@@ -3530,11 +3530,11 @@
       </c>
       <c r="C117" s="1"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B118" s="17" t="s">
+      <c r="B118" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C118" s="1"/>

</xml_diff>